<commit_message>
added JulianaCorrea to Chang-Zhang dial
</commit_message>
<xml_diff>
--- a/assignments.xlsx
+++ b/assignments.xlsx
@@ -5,33 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab4c450ce0f9dc95/Documentos/Proyecto profe David/github/Allignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITHUB\Allignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="11_BBB21FD597D9AEFF0B13124A1AE18DB075D0CB69" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{938EAB91-FC5D-488B-B55E-BAAA32688D50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83E573B-DD73-47A2-A813-050B837E1E9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="35">
   <si>
     <t>chang-zhang</t>
   </si>
@@ -133,6 +122,9 @@
   </si>
   <si>
     <t>assigned</t>
+  </si>
+  <si>
+    <t>JulianaCorrea</t>
   </si>
 </sst>
 </file>
@@ -530,19 +522,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -559,7 +553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -572,8 +566,11 @@
       <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -587,7 +584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -601,7 +598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -615,7 +612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -629,7 +626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -643,7 +640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -657,7 +654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -671,7 +668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -685,7 +682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -699,7 +696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -713,7 +710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -727,7 +724,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -741,7 +738,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -755,7 +752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -769,7 +766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -783,7 +780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -797,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -811,7 +808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -825,7 +822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -839,7 +836,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -853,7 +850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -867,7 +864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,7 +878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -895,7 +892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>4</v>
       </c>
@@ -909,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -923,7 +920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -937,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -951,7 +948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -965,7 +962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -979,7 +976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -993,7 +990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1004,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
@@ -1063,7 +1060,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -1119,7 +1116,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>20</v>
       </c>
@@ -1135,5 +1132,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>